<commit_message>
BoM done except for battery
</commit_message>
<xml_diff>
--- a/Lab7/Lab7BoM.xlsx
+++ b/Lab7/Lab7BoM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90D135E-F4C6-4E07-94EA-7598C3080188}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257539D6-E092-4E51-9363-7208CFFB533D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="117">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -79,12 +79,6 @@
     <t>Battery</t>
   </si>
   <si>
-    <t>Header pins for TM4C</t>
-  </si>
-  <si>
-    <t>Header pins for LCD</t>
-  </si>
-  <si>
     <t>Logic Analyzer pins</t>
   </si>
   <si>
@@ -326,6 +320,57 @@
   </si>
   <si>
     <t>Amazon</t>
+  </si>
+  <si>
+    <t>DIODE</t>
+  </si>
+  <si>
+    <t>1N914 diode</t>
+  </si>
+  <si>
+    <t>Fairchild</t>
+  </si>
+  <si>
+    <t>1N914</t>
+  </si>
+  <si>
+    <t>1N914B-ND</t>
+  </si>
+  <si>
+    <t>Header4</t>
+  </si>
+  <si>
+    <t>952-2262-ND</t>
+  </si>
+  <si>
+    <t>M20-9990246</t>
+  </si>
+  <si>
+    <t>Harwin Inc</t>
+  </si>
+  <si>
+    <t>SIL VERTICAL PC TAIL PIN HEADER</t>
+  </si>
+  <si>
+    <t>A1972-ND</t>
+  </si>
+  <si>
+    <t>640445-4</t>
+  </si>
+  <si>
+    <t>TE Connectivity AMP Connectors</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 4POS .156 TIN</t>
+  </si>
+  <si>
+    <t>Karlsson Robotics</t>
+  </si>
+  <si>
+    <t>PRT-11376</t>
+  </si>
+  <si>
+    <t>Header pins for TM4C/LCD (10, female)</t>
   </si>
 </sst>
 </file>
@@ -336,7 +381,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +420,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -396,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -410,11 +467,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,29 +757,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="10" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="23.7109375" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="3"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -773,19 +836,19 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="I4" s="8">
+        <v>94</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" s="7">
         <v>2.5</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <v>4.99</v>
       </c>
       <c r="L4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -793,25 +856,25 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" t="s">
         <v>99</v>
       </c>
-      <c r="E5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>8.76</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="7">
         <v>17.52</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -819,16 +882,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I6" s="5">
         <v>0.85</v>
@@ -838,10 +901,10 @@
         <v>0.85</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -849,19 +912,19 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>0</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -869,19 +932,19 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="H8" s="4">
         <v>358</v>
@@ -894,10 +957,10 @@
         <v>19.96</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -905,22 +968,22 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="I9" s="5">
         <v>3.5</v>
@@ -930,10 +993,10 @@
         <v>3.5</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -944,198 +1007,256 @@
         <v>18</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="G11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="7">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" ref="J12" si="2">A12*I12</f>
+        <v>0.27</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="4">
+        <v>5001</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" ref="J13" si="3">A13*I13</f>
+        <v>0.92</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="7">
+        <v>4.99</v>
+      </c>
+      <c r="J14" s="7">
+        <v>19.98</v>
+      </c>
+      <c r="L14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.27</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" ref="J13" si="2">A13*I13</f>
-        <v>0.27</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" s="6" t="s">
+      <c r="C15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="4">
-        <v>5001</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0.23</v>
-      </c>
-      <c r="J14" s="5">
-        <f t="shared" ref="J14" si="3">A14*I14</f>
-        <v>0.23</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>93</v>
-      </c>
-      <c r="E15" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" s="8">
-        <v>4.99</v>
-      </c>
-      <c r="J15" s="8">
-        <v>19.98</v>
-      </c>
-      <c r="L15" t="s">
-        <v>42</v>
+      <c r="H15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="5">
+        <v>2.4E-2</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" ref="J15:J18" si="4">A15*I15</f>
+        <v>2.4E-2</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
-        <v>70</v>
+      <c r="C16" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>65</v>
+        <v>73</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>66</v>
+        <v>34</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="I16" s="5">
-        <v>2.4E-2</v>
+        <v>0.26</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" ref="J16:J17" si="4">A16*I16</f>
-        <v>2.4E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.26</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>75</v>
+        <v>3</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>35</v>
+        <v>108</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>77</v>
+        <v>34</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="I17" s="5">
-        <v>0.26</v>
+        <v>0.11</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" si="4"/>
+        <v>0.33</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="I18" s="5">
         <v>0.26</v>
       </c>
-      <c r="K17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
+      <c r="J18" s="5">
+        <f t="shared" si="4"/>
+        <v>0.52</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1143,22 +1264,22 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="I19" s="5">
         <v>0.86</v>
@@ -1168,10 +1289,10 @@
         <v>0.86</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1179,22 +1300,22 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="G20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="I20" s="5">
         <v>0.28999999999999998</v>
@@ -1204,10 +1325,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1215,67 +1336,67 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="G21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="I21" s="5">
         <v>0.19</v>
       </c>
       <c r="J21" s="5">
         <f>A22*I21</f>
-        <v>0.19</v>
+        <v>0.38</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I22" s="5">
         <v>0.31680000000000003</v>
       </c>
       <c r="J22" s="5">
         <f>A22*I22</f>
-        <v>0.31680000000000003</v>
+        <v>0.63360000000000005</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1283,35 +1404,35 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="G23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="I23" s="5">
         <v>0.47</v>
       </c>
       <c r="J23" s="5">
-        <f t="shared" ref="J23:J24" si="6">A23*I23</f>
+        <f t="shared" ref="J23:J25" si="6">A23*I23</f>
         <v>0.47</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -1319,22 +1440,22 @@
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="H24" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I24" s="5">
         <v>7.5</v>
@@ -1344,10 +1465,46 @@
         <v>7.5</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BoM datasheets + currents
</commit_message>
<xml_diff>
--- a/Lab7/Lab7BoM.xlsx
+++ b/Lab7/Lab7BoM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257539D6-E092-4E51-9363-7208CFFB533D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280F56BA-9569-4A3A-9DEA-9F9095171DA2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="145">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -76,9 +76,6 @@
     <t>NRF24L01 RF Module</t>
   </si>
   <si>
-    <t>Battery</t>
-  </si>
-  <si>
     <t>Logic Analyzer pins</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>516-1327-ND</t>
   </si>
   <si>
-    <t>Tantalum, 20V, 10%, 1 uF</t>
-  </si>
-  <si>
     <t>478-1833-ND</t>
   </si>
   <si>
@@ -217,9 +211,6 @@
     <t>1.0KEBK-ND</t>
   </si>
   <si>
-    <t>Carbon 1/6W, 5%</t>
-  </si>
-  <si>
     <t>ASM</t>
   </si>
   <si>
@@ -371,6 +362,99 @@
   </si>
   <si>
     <t>Header pins for TM4C/LCD (10, female)</t>
+  </si>
+  <si>
+    <t>Current Drawn</t>
+  </si>
+  <si>
+    <t>Datasheets</t>
+  </si>
+  <si>
+    <t>13.5 mA</t>
+  </si>
+  <si>
+    <t>Tantalum, 20V, 10%, 4.7 uF</t>
+  </si>
+  <si>
+    <t>Carbon 1/6W, 5%, 470ohm</t>
+  </si>
+  <si>
+    <t>Battery 12V</t>
+  </si>
+  <si>
+    <t>http://docs-europe.electrocomponents.com/webdocs/1009/0900766b810093cc.pdf</t>
+  </si>
+  <si>
+    <t>https://www.vishay.com/docs/40002/293d.pdf</t>
+  </si>
+  <si>
+    <t>http://www.symmetron.ru/suppliers/hirose/files/pdf/hirose/hirose_ZX.pdf</t>
+  </si>
+  <si>
+    <t>http://www.displayfuture.com/Display/datasheet/controller/ST7735.pdf</t>
+  </si>
+  <si>
+    <t>50 mA</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/60/ksc-965385.pdf</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/datasheets/IR333_A_datasheet.pdf</t>
+  </si>
+  <si>
+    <t>http://datasheet.octopart.com/5002-Keystone-datasheet-7266429.pdf</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/lit/ds/symlink/lp2951-n.pdf</t>
+  </si>
+  <si>
+    <t>http://www.onsemi.com/pub/Collateral/1N914-D.PDF</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/datasheets/Components/SMD/nRF24L01Pluss_Preliminary_Product_Specification_v1_0.pdf</t>
+  </si>
+  <si>
+    <t>https://www.tsukasa-d.co.jp/en/data_download/english_catalogue.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ds/2/833/Rocker_SR_PPR-1075680.pdf</t>
+  </si>
+  <si>
+    <t>http://users.ece.utexas.edu/~valvano/Datasheets/L293d.pdf</t>
+  </si>
+  <si>
+    <t>http://www.analog.com/media/en/technical-documentation/obsolete-data-sheets/ADXL210.pdf (obsolete?)</t>
+  </si>
+  <si>
+    <t>0.6 mA</t>
+  </si>
+  <si>
+    <t>200 mA ?</t>
+  </si>
+  <si>
+    <t>13 mA</t>
+  </si>
+  <si>
+    <t>120 / 420 mA ?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>0.35 mA ?</t>
+  </si>
+  <si>
+    <t>100 mA</t>
+  </si>
+  <si>
+    <t>100 mA (Output)</t>
+  </si>
+  <si>
+    <t>0.5 uA ?</t>
+  </si>
+  <si>
+    <t>100 mA ?</t>
   </si>
 </sst>
 </file>
@@ -469,14 +553,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,20 +858,22 @@
     <col min="11" max="11" width="23.7109375" customWidth="1"/>
     <col min="12" max="12" width="12.140625" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="111.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="3"/>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -827,8 +913,14 @@
       <c r="M3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -836,10 +928,13 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
+      </c>
+      <c r="G4" t="s">
+        <v>96</v>
       </c>
       <c r="I4" s="7">
         <v>2.5</v>
@@ -848,24 +943,30 @@
         <v>4.99</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="N4" t="s">
+        <v>116</v>
+      </c>
+      <c r="O4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" t="s">
         <v>96</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" t="s">
-        <v>99</v>
       </c>
       <c r="I5" s="7">
         <v>8.76</v>
@@ -874,24 +975,30 @@
         <v>17.52</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="N5" t="s">
+        <v>138</v>
+      </c>
+      <c r="O5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="I6" s="5">
         <v>0.85</v>
@@ -901,18 +1008,24 @@
         <v>0.85</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="N6" t="s">
+        <v>139</v>
+      </c>
+      <c r="O6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -924,27 +1037,27 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="H8" s="4">
         <v>358</v>
@@ -957,33 +1070,39 @@
         <v>19.96</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="N8" t="s">
+        <v>124</v>
+      </c>
+      <c r="O8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I9" s="5">
         <v>3.5</v>
@@ -993,35 +1112,41 @@
         <v>3.5</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="N9" t="s">
+        <v>137</v>
+      </c>
+      <c r="O9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="I11" s="7">
         <v>0.5</v>
@@ -1030,27 +1155,27 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="F12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="I12" s="5">
         <v>0.27</v>
@@ -1060,33 +1185,33 @@
         <v>0.27</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F13" s="4">
         <v>5001</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I13" s="5">
         <v>0.23</v>
@@ -1096,24 +1221,30 @@
         <v>0.92</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="N13" t="s">
+        <v>139</v>
+      </c>
+      <c r="O13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I14" s="7">
         <v>4.99</v>
@@ -1122,30 +1253,30 @@
         <v>19.98</v>
       </c>
       <c r="L14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="E15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="I15" s="5">
         <v>2.4E-2</v>
@@ -1155,33 +1286,39 @@
         <v>2.4E-2</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="N15" t="s">
+        <v>140</v>
+      </c>
+      <c r="O15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="F16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="H16" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I16" s="5">
         <v>0.26</v>
@@ -1191,31 +1328,31 @@
         <v>0.26</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="10" t="s">
-        <v>109</v>
+      <c r="D17" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>106</v>
+        <v>33</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>103</v>
       </c>
       <c r="I17" s="5">
         <v>0.11</v>
@@ -1225,28 +1362,28 @@
         <v>0.33</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>113</v>
+      <c r="D18" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="E18" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>110</v>
+        <v>33</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="I18" s="5">
         <v>0.26</v>
@@ -1256,30 +1393,30 @@
         <v>0.52</v>
       </c>
       <c r="K18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="F19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="I19" s="5">
         <v>0.86</v>
@@ -1289,33 +1426,39 @@
         <v>0.86</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="N19" t="s">
+        <v>124</v>
+      </c>
+      <c r="O19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="I20" s="5">
         <v>0.28999999999999998</v>
@@ -1325,101 +1468,119 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="N20" t="s">
+        <v>141</v>
+      </c>
+      <c r="O20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="I21" s="5">
         <v>0.19</v>
       </c>
       <c r="J21" s="5">
-        <f>A22*I21</f>
-        <v>0.38</v>
+        <f>A21*I21</f>
+        <v>0.19</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="N21" t="s">
+        <v>142</v>
+      </c>
+      <c r="O21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I22" s="5">
         <v>0.31680000000000003</v>
       </c>
       <c r="J22" s="5">
         <f>A22*I22</f>
-        <v>0.63360000000000005</v>
+        <v>0.95040000000000013</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="N22" t="s">
+        <v>143</v>
+      </c>
+      <c r="O22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="I23" s="5">
         <v>0.47</v>
@@ -1429,33 +1590,39 @@
         <v>0.47</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="N23" t="s">
+        <v>144</v>
+      </c>
+      <c r="O23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="H24" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I24" s="5">
         <v>7.5</v>
@@ -1465,33 +1632,39 @@
         <v>7.5</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="N24" t="s">
+        <v>135</v>
+      </c>
+      <c r="O24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="G25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="I25" s="5">
         <v>0.05</v>
@@ -1501,10 +1674,16 @@
         <v>0.1</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="N25" t="s">
+        <v>136</v>
+      </c>
+      <c r="O25" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>